<commit_message>
Ordner für Übungen für Kurs FIAE B
</commit_message>
<xml_diff>
--- a/Netzplan_Übung_Gantt.xlsx
+++ b/Netzplan_Übung_Gantt.xlsx
@@ -271,7 +271,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -297,6 +297,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2168,9 +2172,9 @@
   <dimension ref="A1:BV67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="0" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <pane xSplit="9" ySplit="0" topLeftCell="AG1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J5" activeCellId="0" sqref="J5"/>
+      <selection pane="topRight" activeCell="A13" activeCellId="0" sqref="13:13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.83203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2410,18 +2414,47 @@
       </c>
       <c r="I2" s="6" t="n">
         <f aca="false">SUM(J2:CV2)</f>
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="J2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
@@ -2432,18 +2465,59 @@
       </c>
       <c r="I3" s="6" t="n">
         <f aca="false">SUM(J3:CV3)</f>
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="7"/>
+      <c r="AH3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2456,18 +2530,59 @@
       </c>
       <c r="I4" s="6" t="n">
         <f aca="false">SUM(J4:CV4)</f>
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
@@ -2478,18 +2593,55 @@
       </c>
       <c r="I5" s="6" t="n">
         <f aca="false">SUM(J5:CV5)</f>
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
@@ -2500,18 +2652,59 @@
       </c>
       <c r="I6" s="6" t="n">
         <f aca="false">SUM(J6:CV6)</f>
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
@@ -2522,20 +2715,61 @@
       </c>
       <c r="I7" s="6" t="n">
         <f aca="false">SUM(J7:CV7)</f>
-        <v>0</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
@@ -2548,18 +2782,63 @@
       </c>
       <c r="I8" s="6" t="n">
         <f aca="false">SUM(J8:CV8)</f>
-        <v>0</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="7"/>
+      <c r="AT8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="5" t="s">
         <v>4</v>
       </c>
@@ -2570,18 +2849,60 @@
       </c>
       <c r="I9" s="6" t="n">
         <f aca="false">SUM(J9:CV9)</f>
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="5" t="s">
         <v>4</v>
       </c>
@@ -2592,18 +2913,57 @@
       </c>
       <c r="I10" s="6" t="n">
         <f aca="false">SUM(J10:CV10)</f>
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2614,20 +2974,69 @@
       </c>
       <c r="I11" s="6" t="n">
         <f aca="false">SUM(J11:CV11)</f>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AM11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV11" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
@@ -2638,20 +3047,51 @@
       </c>
       <c r="I12" s="6" t="n">
         <f aca="false">SUM(J12:CV12)</f>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AR12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -2660,679 +3100,716 @@
       </c>
       <c r="I13" s="6" t="n">
         <f aca="false">SUM(J13:CV13)</f>
+        <v>4</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AY13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10" t="n">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="n">
         <f aca="false">A15+A17</f>
         <v>2</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="9" t="n">
         <f aca="false">C15</f>
         <v>2</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10" t="n">
+      <c r="G15" s="10"/>
+      <c r="H15" s="11" t="n">
         <f aca="false">F15+F17</f>
         <v>10</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="9" t="n">
         <f aca="false">H15</f>
         <v>10</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="10" t="n">
+      <c r="L15" s="10"/>
+      <c r="M15" s="11" t="n">
         <f aca="false">K15+K17</f>
         <v>16</v>
       </c>
-      <c r="P15" s="8" t="n">
+      <c r="P15" s="9" t="n">
         <f aca="false">M15</f>
         <v>16</v>
       </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="10" t="n">
+      <c r="Q15" s="10"/>
+      <c r="R15" s="11" t="n">
         <f aca="false">P15+P17</f>
         <v>21</v>
       </c>
-      <c r="U15" s="8" t="n">
+      <c r="U15" s="9" t="n">
         <f aca="false">R15</f>
         <v>21</v>
       </c>
-      <c r="V15" s="9"/>
-      <c r="W15" s="10" t="n">
+      <c r="V15" s="10"/>
+      <c r="W15" s="11" t="n">
         <f aca="false">U15+U17</f>
         <v>29</v>
       </c>
-      <c r="Z15" s="8" t="n">
+      <c r="Z15" s="9" t="n">
         <f aca="false">MAX(W15,W20)</f>
         <v>29</v>
       </c>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="10" t="n">
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="11" t="n">
         <f aca="false">Z15+Z17</f>
         <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="F16" s="11" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="F16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="K16" s="11" t="s">
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="K16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="P16" s="11" t="s">
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="P16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="U16" s="11" t="s">
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="U16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="Z16" s="11" t="s">
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="Z16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="n">
+      <c r="A17" s="13" t="n">
         <f aca="false">H2</f>
         <v>2</v>
       </c>
-      <c r="B17" s="13" t="n">
+      <c r="B17" s="14" t="n">
         <f aca="false">C18-C15</f>
         <v>0</v>
       </c>
-      <c r="C17" s="13" t="n">
+      <c r="C17" s="14" t="n">
         <f aca="false">MIN(F15,F20)-C15</f>
         <v>0</v>
       </c>
-      <c r="F17" s="12" t="n">
+      <c r="F17" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="G17" s="13" t="n">
+      <c r="G17" s="14" t="n">
         <f aca="false">H18-H15</f>
         <v>0</v>
       </c>
-      <c r="H17" s="13" t="n">
+      <c r="H17" s="14" t="n">
         <f aca="false">K15-H15</f>
         <v>0</v>
       </c>
-      <c r="K17" s="12" t="n">
+      <c r="K17" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="L17" s="13" t="n">
+      <c r="L17" s="14" t="n">
         <f aca="false">M18-M15</f>
         <v>0</v>
       </c>
-      <c r="M17" s="13" t="n">
+      <c r="M17" s="14" t="n">
         <f aca="false">P15-M15</f>
         <v>0</v>
       </c>
-      <c r="P17" s="12" t="n">
+      <c r="P17" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="Q17" s="13" t="n">
+      <c r="Q17" s="14" t="n">
         <f aca="false">R18-R15</f>
         <v>0</v>
       </c>
-      <c r="R17" s="13" t="n">
+      <c r="R17" s="14" t="n">
         <f aca="false">U15-R15</f>
         <v>0</v>
       </c>
-      <c r="U17" s="12" t="n">
+      <c r="U17" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="V17" s="13" t="n">
+      <c r="V17" s="14" t="n">
         <f aca="false">W18-W15</f>
         <v>0</v>
       </c>
-      <c r="W17" s="13" t="n">
+      <c r="W17" s="14" t="n">
         <f aca="false">Z15-W15</f>
         <v>0</v>
       </c>
-      <c r="Z17" s="12" t="n">
+      <c r="Z17" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="AA17" s="13" t="n">
+      <c r="AA17" s="14" t="n">
         <f aca="false">AB18-AB15</f>
         <v>0</v>
       </c>
-      <c r="AB17" s="13"/>
+      <c r="AB17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="15" t="n">
         <f aca="false">C18-A17</f>
         <v>0</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="n">
+      <c r="B18" s="16"/>
+      <c r="C18" s="17" t="n">
         <f aca="false">MIN(F18,F23)</f>
         <v>2</v>
       </c>
-      <c r="F18" s="14" t="n">
+      <c r="F18" s="15" t="n">
         <f aca="false">H18-F17</f>
         <v>2</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16" t="n">
+      <c r="G18" s="16"/>
+      <c r="H18" s="17" t="n">
         <f aca="false">K18</f>
         <v>10</v>
       </c>
-      <c r="K18" s="14" t="n">
+      <c r="K18" s="15" t="n">
         <f aca="false">M18-K17</f>
         <v>10</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16" t="n">
+      <c r="L18" s="16"/>
+      <c r="M18" s="17" t="n">
         <f aca="false">P18</f>
         <v>16</v>
       </c>
-      <c r="P18" s="14" t="n">
+      <c r="P18" s="15" t="n">
         <f aca="false">R18-P17</f>
         <v>16</v>
       </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="16" t="n">
+      <c r="Q18" s="16"/>
+      <c r="R18" s="17" t="n">
         <f aca="false">U18</f>
         <v>21</v>
       </c>
-      <c r="U18" s="14" t="n">
+      <c r="U18" s="15" t="n">
         <f aca="false">W18-U17</f>
         <v>21</v>
       </c>
-      <c r="V18" s="15"/>
-      <c r="W18" s="16" t="n">
+      <c r="V18" s="16"/>
+      <c r="W18" s="17" t="n">
         <f aca="false">Z18</f>
         <v>29</v>
       </c>
-      <c r="Z18" s="14" t="n">
+      <c r="Z18" s="15" t="n">
         <f aca="false">AB18-Z17</f>
         <v>29</v>
       </c>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="16" t="n">
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="17" t="n">
         <f aca="false">AB15</f>
         <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="8" t="n">
+      <c r="F20" s="9" t="n">
         <f aca="false">C15</f>
         <v>2</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="10" t="n">
+      <c r="G20" s="10"/>
+      <c r="H20" s="11" t="n">
         <f aca="false">F20+F22</f>
         <v>10</v>
       </c>
-      <c r="K20" s="8" t="n">
+      <c r="K20" s="9" t="n">
         <f aca="false">H20</f>
         <v>10</v>
       </c>
-      <c r="L20" s="9"/>
-      <c r="M20" s="10" t="n">
+      <c r="L20" s="10"/>
+      <c r="M20" s="11" t="n">
         <f aca="false">K20+K22</f>
         <v>18</v>
       </c>
-      <c r="P20" s="8" t="n">
+      <c r="P20" s="9" t="n">
         <f aca="false">M20</f>
         <v>18</v>
       </c>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="10" t="n">
+      <c r="Q20" s="10"/>
+      <c r="R20" s="11" t="n">
         <f aca="false">P20+P22</f>
         <v>24</v>
       </c>
-      <c r="U20" s="8" t="n">
+      <c r="U20" s="9" t="n">
         <f aca="false">MAX(R20,R25)</f>
         <v>24</v>
       </c>
-      <c r="V20" s="9"/>
-      <c r="W20" s="10" t="n">
+      <c r="V20" s="10"/>
+      <c r="W20" s="11" t="n">
         <f aca="false">U20+U22</f>
         <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="K21" s="11" t="s">
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="K21" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="P21" s="11" t="s">
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="P21" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="U21" s="11" t="s">
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="U21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="12" t="n">
+      <c r="F22" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="G22" s="13" t="n">
+      <c r="G22" s="14" t="n">
         <f aca="false">H23-H20</f>
         <v>3</v>
       </c>
-      <c r="H22" s="13" t="n">
+      <c r="H22" s="14" t="n">
         <f aca="false">MIN(K20,K25)-H20</f>
         <v>0</v>
       </c>
-      <c r="K22" s="12" t="n">
+      <c r="K22" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="L22" s="13" t="n">
+      <c r="L22" s="14" t="n">
         <f aca="false">M23-M20</f>
         <v>3</v>
       </c>
-      <c r="M22" s="13" t="n">
+      <c r="M22" s="14" t="n">
         <f aca="false">P20-M20</f>
         <v>0</v>
       </c>
-      <c r="P22" s="12" t="n">
+      <c r="P22" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="Q22" s="13" t="n">
+      <c r="Q22" s="14" t="n">
         <f aca="false">R23-R20</f>
         <v>3</v>
       </c>
-      <c r="R22" s="13" t="n">
+      <c r="R22" s="14" t="n">
         <f aca="false">U20-R20</f>
         <v>0</v>
       </c>
-      <c r="U22" s="12" t="n">
+      <c r="U22" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="V22" s="13" t="n">
+      <c r="V22" s="14" t="n">
         <f aca="false">W23-W20</f>
         <v>3</v>
       </c>
-      <c r="W22" s="13" t="n">
+      <c r="W22" s="14" t="n">
         <f aca="false">Z15-W20</f>
         <v>3</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="14" t="n">
+      <c r="F23" s="15" t="n">
         <f aca="false">H23-F22</f>
         <v>5</v>
       </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16" t="n">
+      <c r="G23" s="16"/>
+      <c r="H23" s="17" t="n">
         <f aca="false">MIN(K23,K28)</f>
         <v>13</v>
       </c>
-      <c r="K23" s="14" t="n">
+      <c r="K23" s="15" t="n">
         <f aca="false">M23-K22</f>
         <v>13</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="16" t="n">
+      <c r="L23" s="16"/>
+      <c r="M23" s="17" t="n">
         <f aca="false">P23</f>
         <v>21</v>
       </c>
-      <c r="P23" s="14" t="n">
+      <c r="P23" s="15" t="n">
         <f aca="false">R23-P22</f>
         <v>21</v>
       </c>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="16" t="n">
+      <c r="Q23" s="16"/>
+      <c r="R23" s="17" t="n">
         <f aca="false">U23</f>
         <v>27</v>
       </c>
-      <c r="U23" s="14" t="n">
+      <c r="U23" s="15" t="n">
         <f aca="false">W23-U22</f>
         <v>27</v>
       </c>
-      <c r="V23" s="15"/>
-      <c r="W23" s="16" t="n">
+      <c r="V23" s="16"/>
+      <c r="W23" s="17" t="n">
         <f aca="false">Z18</f>
         <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K25" s="8" t="n">
+      <c r="K25" s="9" t="n">
         <f aca="false">H20</f>
         <v>10</v>
       </c>
-      <c r="L25" s="9"/>
-      <c r="M25" s="10" t="n">
+      <c r="L25" s="10"/>
+      <c r="M25" s="11" t="n">
         <f aca="false">K25+K27</f>
         <v>18</v>
       </c>
-      <c r="P25" s="8" t="n">
+      <c r="P25" s="9" t="n">
         <f aca="false">M25</f>
         <v>18</v>
       </c>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="10" t="n">
+      <c r="Q25" s="10"/>
+      <c r="R25" s="11" t="n">
         <f aca="false">P25+P27</f>
         <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K26" s="11" t="s">
+      <c r="K26" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="P26" s="11" t="s">
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="P26" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="12" t="n">
+      <c r="K27" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="L27" s="13" t="n">
+      <c r="L27" s="14" t="n">
         <f aca="false">M28-M25</f>
         <v>4</v>
       </c>
-      <c r="M27" s="13" t="n">
+      <c r="M27" s="14" t="n">
         <f aca="false">P25-M25</f>
         <v>0</v>
       </c>
-      <c r="P27" s="12" t="n">
+      <c r="P27" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="Q27" s="13" t="n">
+      <c r="Q27" s="14" t="n">
         <f aca="false">R28-R25</f>
         <v>4</v>
       </c>
-      <c r="R27" s="13" t="n">
+      <c r="R27" s="14" t="n">
         <f aca="false">U20-R25</f>
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="14" t="n">
+      <c r="K28" s="15" t="n">
         <f aca="false">M28-K27</f>
         <v>14</v>
       </c>
-      <c r="L28" s="15"/>
-      <c r="M28" s="16" t="n">
+      <c r="L28" s="16"/>
+      <c r="M28" s="17" t="n">
         <f aca="false">P28</f>
         <v>22</v>
       </c>
-      <c r="P28" s="14" t="n">
+      <c r="P28" s="15" t="n">
         <f aca="false">R28-P27</f>
         <v>22</v>
       </c>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="16" t="n">
+      <c r="Q28" s="16"/>
+      <c r="R28" s="17" t="n">
         <f aca="false">U23</f>
         <v>27</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="17"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18"/>
+      <c r="A54" s="18"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="17"/>
-      <c r="B55" s="19" t="s">
+      <c r="A55" s="18"/>
+      <c r="B55" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19" t="s">
+      <c r="C55" s="20"/>
+      <c r="D55" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="18"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="17"/>
-      <c r="B56" s="20" t="s">
+      <c r="A56" s="18"/>
+      <c r="B56" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="21" t="s">
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="18"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="17"/>
-      <c r="B57" s="22" t="s">
+      <c r="A57" s="18"/>
+      <c r="B57" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="23" t="s">
+      <c r="C57" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="18"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="17"/>
-      <c r="B58" s="19" t="s">
+      <c r="A58" s="18"/>
+      <c r="B58" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19" t="s">
+      <c r="C58" s="20"/>
+      <c r="D58" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="18"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="17"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="18"/>
+      <c r="A59" s="18"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="20"/>
+      <c r="L59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="17"/>
-      <c r="B60" s="24" t="s">
+      <c r="A60" s="18"/>
+      <c r="B60" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="25" t="s">
+      <c r="C60" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-      <c r="H60" s="25"/>
-      <c r="I60" s="25"/>
-      <c r="J60" s="25"/>
-      <c r="K60" s="25"/>
-      <c r="L60" s="18"/>
+      <c r="D60" s="26"/>
+      <c r="E60" s="26"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="26"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+      <c r="L60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="17"/>
-      <c r="B61" s="24" t="s">
+      <c r="A61" s="18"/>
+      <c r="B61" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="25" t="s">
+      <c r="C61" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-      <c r="H61" s="25"/>
-      <c r="I61" s="25"/>
-      <c r="J61" s="25"/>
-      <c r="K61" s="25"/>
-      <c r="L61" s="18"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="17"/>
-      <c r="B62" s="24" t="s">
+      <c r="A62" s="18"/>
+      <c r="B62" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="25" t="s">
+      <c r="C62" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-      <c r="H62" s="25"/>
-      <c r="I62" s="25"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="25"/>
-      <c r="L62" s="18"/>
+      <c r="D62" s="26"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="26"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+      <c r="L62" s="19"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="17"/>
-      <c r="B63" s="24" t="s">
+      <c r="A63" s="18"/>
+      <c r="B63" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="25" t="s">
+      <c r="C63" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
-      <c r="J63" s="25"/>
-      <c r="K63" s="25"/>
-      <c r="L63" s="18"/>
+      <c r="D63" s="26"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="26"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="26"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="26"/>
+      <c r="K63" s="26"/>
+      <c r="L63" s="19"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="17"/>
-      <c r="B64" s="22" t="s">
+      <c r="A64" s="18"/>
+      <c r="B64" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="25" t="s">
+      <c r="C64" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="25"/>
-      <c r="K64" s="25"/>
-      <c r="L64" s="18"/>
+      <c r="D64" s="26"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="26"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+      <c r="L64" s="19"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="17"/>
-      <c r="B65" s="23" t="s">
+      <c r="A65" s="18"/>
+      <c r="B65" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C65" s="25" t="s">
+      <c r="C65" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
-      <c r="I65" s="25"/>
-      <c r="J65" s="25"/>
-      <c r="K65" s="25"/>
-      <c r="L65" s="18"/>
+      <c r="D65" s="26"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="26"/>
+      <c r="K65" s="26"/>
+      <c r="L65" s="19"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="17"/>
-      <c r="B66" s="26" t="s">
+      <c r="A66" s="18"/>
+      <c r="B66" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="18" t="s">
+      <c r="C66" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
-      <c r="K66" s="18"/>
-      <c r="L66" s="18"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+      <c r="L66" s="19"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="17"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="18"/>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18"/>
+      <c r="A67" s="18"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+      <c r="L67" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -3361,7 +3838,7 @@
   </mergeCells>
   <conditionalFormatting sqref="J1:CF13">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>IF(OR(WEEKDAY(I$1)=7,WEEKDAY(I$1)=1),1,0)</formula>
+      <formula>IF(OR(WEEKDAY(J$1)=7,WEEKDAY(J$1)=1),1,0)</formula>
     </cfRule>
     <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>1</formula>
@@ -3386,7 +3863,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="1" sqref="13:13 C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3434,11 +3911,11 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
@@ -3452,11 +3929,11 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
       <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
@@ -3472,11 +3949,11 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
       <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
@@ -3490,11 +3967,11 @@
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
       <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
@@ -3508,11 +3985,11 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="5" t="s">
         <v>11</v>
       </c>
@@ -3526,13 +4003,13 @@
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
@@ -3548,13 +4025,13 @@
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
@@ -3572,11 +4049,11 @@
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
@@ -3590,13 +4067,13 @@
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
@@ -3610,11 +4087,11 @@
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
@@ -3628,13 +4105,13 @@
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E13" s="5"/>
@@ -3645,441 +4122,441 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="n">
+      <c r="A15" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10" t="n">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="n">
         <f aca="false">A15+A17</f>
         <v>6</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="9" t="n">
         <f aca="false">C15</f>
         <v>6</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10" t="n">
+      <c r="G15" s="10"/>
+      <c r="H15" s="11" t="n">
         <f aca="false">F15+F17</f>
         <v>13</v>
       </c>
-      <c r="K15" s="8" t="n">
+      <c r="K15" s="9" t="n">
         <f aca="false">H15</f>
         <v>13</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="M15" s="10" t="n">
+      <c r="L15" s="10"/>
+      <c r="M15" s="11" t="n">
         <f aca="false">K15+K17</f>
         <v>17</v>
       </c>
-      <c r="P15" s="8" t="n">
+      <c r="P15" s="9" t="n">
         <f aca="false">M15</f>
         <v>17</v>
       </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="10" t="n">
+      <c r="Q15" s="10"/>
+      <c r="R15" s="11" t="n">
         <f aca="false">P15+P17</f>
         <v>20</v>
       </c>
-      <c r="U15" s="8" t="n">
+      <c r="U15" s="9" t="n">
         <f aca="false">MAX(R15,R21)</f>
         <v>24</v>
       </c>
-      <c r="V15" s="9"/>
-      <c r="W15" s="10" t="n">
+      <c r="V15" s="10"/>
+      <c r="W15" s="11" t="n">
         <f aca="false">U15+U17</f>
         <v>32</v>
       </c>
-      <c r="Z15" s="8" t="n">
+      <c r="Z15" s="9" t="n">
         <f aca="false">MAX(W15,W21,W27)</f>
         <v>33</v>
       </c>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="10" t="n">
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="11" t="n">
         <f aca="false">Z15+Z17</f>
         <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="F16" s="11" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="F16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="K16" s="11" t="s">
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="K16" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="P16" s="11" t="s">
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="P16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="U16" s="11" t="s">
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="U16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="Z16" s="11" t="s">
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="Z16" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="n">
+      <c r="A17" s="13" t="n">
         <f aca="false">H2</f>
         <v>6</v>
       </c>
-      <c r="B17" s="13" t="n">
+      <c r="B17" s="14" t="n">
         <f aca="false">C18-C15</f>
         <v>0</v>
       </c>
-      <c r="C17" s="13" t="n">
+      <c r="C17" s="14" t="n">
         <f aca="false">MIN(F15,F21)-C15</f>
         <v>0</v>
       </c>
-      <c r="F17" s="12" t="n">
+      <c r="F17" s="13" t="n">
         <f aca="false">H3</f>
         <v>7</v>
       </c>
-      <c r="G17" s="13" t="n">
+      <c r="G17" s="14" t="n">
         <f aca="false">H18-H15</f>
         <v>5</v>
       </c>
-      <c r="H17" s="13" t="n">
+      <c r="H17" s="14" t="n">
         <f aca="false">K15-H15</f>
         <v>0</v>
       </c>
-      <c r="K17" s="12" t="n">
+      <c r="K17" s="13" t="n">
         <f aca="false">H5</f>
         <v>4</v>
       </c>
-      <c r="L17" s="13" t="n">
+      <c r="L17" s="14" t="n">
         <f aca="false">M18-M15</f>
         <v>5</v>
       </c>
-      <c r="M17" s="13" t="n">
+      <c r="M17" s="14" t="n">
         <f aca="false">P15-M15</f>
         <v>0</v>
       </c>
-      <c r="P17" s="12" t="n">
+      <c r="P17" s="13" t="n">
         <f aca="false">H8</f>
         <v>3</v>
       </c>
-      <c r="Q17" s="13" t="n">
+      <c r="Q17" s="14" t="n">
         <f aca="false">R18-R15</f>
         <v>5</v>
       </c>
-      <c r="R17" s="13" t="n">
+      <c r="R17" s="14" t="n">
         <f aca="false">U15-R15</f>
         <v>4</v>
       </c>
-      <c r="U17" s="12" t="n">
+      <c r="U17" s="13" t="n">
         <f aca="false">H11</f>
         <v>8</v>
       </c>
-      <c r="V17" s="13" t="n">
+      <c r="V17" s="14" t="n">
         <f aca="false">W18-W15</f>
         <v>1</v>
       </c>
-      <c r="W17" s="13" t="n">
+      <c r="W17" s="14" t="n">
         <f aca="false">Z15-W15</f>
         <v>1</v>
       </c>
-      <c r="Z17" s="12" t="n">
+      <c r="Z17" s="13" t="n">
         <f aca="false">H13</f>
         <v>8</v>
       </c>
-      <c r="AA17" s="13" t="n">
+      <c r="AA17" s="14" t="n">
         <f aca="false">AB18-AB15</f>
         <v>0</v>
       </c>
-      <c r="AB17" s="13"/>
+      <c r="AB17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="15" t="n">
         <f aca="false">C18-A17</f>
         <v>0</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16" t="n">
+      <c r="B18" s="16"/>
+      <c r="C18" s="17" t="n">
         <f aca="false">MIN(F18,F24)</f>
         <v>6</v>
       </c>
-      <c r="F18" s="14" t="n">
+      <c r="F18" s="15" t="n">
         <f aca="false">H18-F17</f>
         <v>11</v>
       </c>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16" t="n">
+      <c r="G18" s="16"/>
+      <c r="H18" s="17" t="n">
         <f aca="false">K18</f>
         <v>18</v>
       </c>
-      <c r="K18" s="14" t="n">
+      <c r="K18" s="15" t="n">
         <f aca="false">M18-K17</f>
         <v>18</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16" t="n">
+      <c r="L18" s="16"/>
+      <c r="M18" s="17" t="n">
         <f aca="false">P18</f>
         <v>22</v>
       </c>
-      <c r="P18" s="14" t="n">
+      <c r="P18" s="15" t="n">
         <f aca="false">R18-P17</f>
         <v>22</v>
       </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="16" t="n">
+      <c r="Q18" s="16"/>
+      <c r="R18" s="17" t="n">
         <f aca="false">U18</f>
         <v>25</v>
       </c>
-      <c r="U18" s="14" t="n">
+      <c r="U18" s="15" t="n">
         <f aca="false">W18-U17</f>
         <v>25</v>
       </c>
-      <c r="V18" s="15"/>
-      <c r="W18" s="16" t="n">
+      <c r="V18" s="16"/>
+      <c r="W18" s="17" t="n">
         <f aca="false">Z18</f>
         <v>33</v>
       </c>
-      <c r="Z18" s="14" t="n">
+      <c r="Z18" s="15" t="n">
         <f aca="false">AB18-Z17</f>
         <v>33</v>
       </c>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="16" t="n">
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="17" t="n">
         <f aca="false">AB15</f>
         <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F21" s="8" t="n">
+      <c r="F21" s="9" t="n">
         <f aca="false">C15</f>
         <v>6</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10" t="n">
+      <c r="G21" s="10"/>
+      <c r="H21" s="11" t="n">
         <f aca="false">F21+F23</f>
         <v>13</v>
       </c>
-      <c r="K21" s="8" t="n">
+      <c r="K21" s="9" t="n">
         <f aca="false">H21</f>
         <v>13</v>
       </c>
-      <c r="L21" s="9"/>
-      <c r="M21" s="10" t="n">
+      <c r="L21" s="10"/>
+      <c r="M21" s="11" t="n">
         <f aca="false">K21+K23</f>
         <v>17</v>
       </c>
-      <c r="P21" s="8" t="n">
+      <c r="P21" s="9" t="n">
         <f aca="false">MAX(M21,M27)</f>
         <v>18</v>
       </c>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="10" t="n">
+      <c r="Q21" s="10"/>
+      <c r="R21" s="11" t="n">
         <f aca="false">P21+P23</f>
         <v>24</v>
       </c>
-      <c r="U21" s="8" t="n">
+      <c r="U21" s="9" t="n">
         <f aca="false">R21</f>
         <v>24</v>
       </c>
-      <c r="V21" s="9"/>
-      <c r="W21" s="10" t="n">
+      <c r="V21" s="10"/>
+      <c r="W21" s="11" t="n">
         <f aca="false">U21+U23</f>
         <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="K22" s="11" t="s">
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="K22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="P22" s="11" t="s">
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="P22" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="U22" s="11" t="s">
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="U22" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="12" t="n">
+      <c r="F23" s="13" t="n">
         <f aca="false">H4</f>
         <v>7</v>
       </c>
-      <c r="G23" s="13" t="n">
+      <c r="G23" s="14" t="n">
         <f aca="false">H24-H21</f>
         <v>0</v>
       </c>
-      <c r="H23" s="13" t="n">
+      <c r="H23" s="14" t="n">
         <f aca="false">MIN(K21,K27)-H21</f>
         <v>0</v>
       </c>
-      <c r="K23" s="12" t="n">
+      <c r="K23" s="13" t="n">
         <f aca="false">H6</f>
         <v>4</v>
       </c>
-      <c r="L23" s="13" t="n">
+      <c r="L23" s="14" t="n">
         <f aca="false">M24-M21</f>
         <v>1</v>
       </c>
-      <c r="M23" s="13" t="n">
+      <c r="M23" s="14" t="n">
         <f aca="false">P21-M21</f>
         <v>1</v>
       </c>
-      <c r="P23" s="12" t="n">
+      <c r="P23" s="13" t="n">
         <f aca="false">H9</f>
         <v>6</v>
       </c>
-      <c r="Q23" s="13" t="n">
+      <c r="Q23" s="14" t="n">
         <f aca="false">R24-R21</f>
         <v>0</v>
       </c>
-      <c r="R23" s="13" t="n">
+      <c r="R23" s="14" t="n">
         <f aca="false">MIN(U15,U21,U27)-R21</f>
         <v>0</v>
       </c>
-      <c r="U23" s="12" t="n">
+      <c r="U23" s="13" t="n">
         <f aca="false">H10</f>
         <v>2</v>
       </c>
-      <c r="V23" s="13" t="n">
+      <c r="V23" s="14" t="n">
         <f aca="false">W24-W21</f>
         <v>7</v>
       </c>
-      <c r="W23" s="13" t="n">
+      <c r="W23" s="14" t="n">
         <f aca="false">Z15-W21</f>
         <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F24" s="14" t="n">
+      <c r="F24" s="15" t="n">
         <f aca="false">H24-F23</f>
         <v>6</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16" t="n">
+      <c r="G24" s="16"/>
+      <c r="H24" s="17" t="n">
         <f aca="false">MIN(K24,K30)</f>
         <v>13</v>
       </c>
-      <c r="K24" s="14" t="n">
+      <c r="K24" s="15" t="n">
         <f aca="false">M24-K23</f>
         <v>14</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="16" t="n">
+      <c r="L24" s="16"/>
+      <c r="M24" s="17" t="n">
         <f aca="false">P24</f>
         <v>18</v>
       </c>
-      <c r="P24" s="14" t="n">
+      <c r="P24" s="15" t="n">
         <f aca="false">R24-P23</f>
         <v>18</v>
       </c>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="16" t="n">
+      <c r="Q24" s="16"/>
+      <c r="R24" s="17" t="n">
         <f aca="false">MIN(U18,U24,U30)</f>
         <v>24</v>
       </c>
-      <c r="U24" s="14" t="n">
+      <c r="U24" s="15" t="n">
         <f aca="false">W24-U23</f>
         <v>31</v>
       </c>
-      <c r="V24" s="15"/>
-      <c r="W24" s="16" t="n">
+      <c r="V24" s="16"/>
+      <c r="W24" s="17" t="n">
         <f aca="false">Z18</f>
         <v>33</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="8" t="n">
+      <c r="K27" s="9" t="n">
         <f aca="false">H21</f>
         <v>13</v>
       </c>
-      <c r="L27" s="9"/>
-      <c r="M27" s="10" t="n">
+      <c r="L27" s="10"/>
+      <c r="M27" s="11" t="n">
         <f aca="false">K27+K29</f>
         <v>18</v>
       </c>
-      <c r="U27" s="8" t="n">
+      <c r="U27" s="9" t="n">
         <f aca="false">R21</f>
         <v>24</v>
       </c>
-      <c r="V27" s="9"/>
-      <c r="W27" s="10" t="n">
+      <c r="V27" s="10"/>
+      <c r="W27" s="11" t="n">
         <f aca="false">U27+U29</f>
         <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K28" s="11" t="s">
+      <c r="K28" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="U28" s="11" t="s">
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="U28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
+      <c r="V28" s="12"/>
+      <c r="W28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K29" s="12" t="n">
+      <c r="K29" s="13" t="n">
         <f aca="false">H7</f>
         <v>5</v>
       </c>
-      <c r="L29" s="13" t="n">
+      <c r="L29" s="14" t="n">
         <f aca="false">M30-M27</f>
         <v>0</v>
       </c>
-      <c r="M29" s="13" t="n">
+      <c r="M29" s="14" t="n">
         <f aca="false">P21-M27</f>
         <v>0</v>
       </c>
-      <c r="U29" s="12" t="n">
+      <c r="U29" s="13" t="n">
         <f aca="false">H12</f>
         <v>9</v>
       </c>
-      <c r="V29" s="13" t="n">
+      <c r="V29" s="14" t="n">
         <f aca="false">W30-W27</f>
         <v>0</v>
       </c>
-      <c r="W29" s="13" t="n">
+      <c r="W29" s="14" t="n">
         <f aca="false">Z15-W27</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K30" s="14" t="n">
+      <c r="K30" s="15" t="n">
         <f aca="false">M30-K29</f>
         <v>13</v>
       </c>
-      <c r="L30" s="15"/>
-      <c r="M30" s="16" t="n">
+      <c r="L30" s="16"/>
+      <c r="M30" s="17" t="n">
         <f aca="false">P24</f>
         <v>18</v>
       </c>
-      <c r="U30" s="14" t="n">
+      <c r="U30" s="15" t="n">
         <f aca="false">W30-U29</f>
         <v>24</v>
       </c>
-      <c r="V30" s="15"/>
-      <c r="W30" s="16" t="n">
+      <c r="V30" s="16"/>
+      <c r="W30" s="17" t="n">
         <f aca="false">Z18</f>
         <v>33</v>
       </c>

</xml_diff>